<commit_message>
Ephyz unit tests in DB
</commit_message>
<xml_diff>
--- a/ephyz/circuit-level-behaviors.xlsx
+++ b/ephyz/circuit-level-behaviors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.162.132\Repositories\OlfactoryBulb\ephyz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\OlfactoryBulb\ephyz\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Paper</t>
   </si>
@@ -130,6 +131,39 @@
   </si>
   <si>
     <t>Suggests the MC-&gt;GC synapse causes long lasting calcium currents</t>
+  </si>
+  <si>
+    <t>GC</t>
+  </si>
+  <si>
+    <t>ADP amplitude</t>
+  </si>
+  <si>
+    <t>11.1+-4.7 mV</t>
+  </si>
+  <si>
+    <t>not REPORTED</t>
+  </si>
+  <si>
+    <t>Soma injections 1000pa for 1ms. a mean sAP-ADP amplitude above resting potential</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>ADP half-duration</t>
+  </si>
+  <si>
+    <t>42+-22 ms</t>
+  </si>
+  <si>
+    <t>Soma injections 1000pa for 1ms</t>
+  </si>
+  <si>
+    <t>Throughout the paper, tau1/2 denotes halfdurations from the peak amplitude of Vm onward, measured between the onset of the afterdepolarization (ADP) right after the sodium spike and one-half of its maximum amplitude</t>
+  </si>
+  <si>
+    <t>GCs show ADPs in vivo to somatic stimulation, and LLDs to glomerular stimulation</t>
   </si>
 </sst>
 </file>
@@ -448,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +626,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -607,6 +641,81 @@
       </c>
       <c r="E18" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22">
+        <v>49</v>
+      </c>
+      <c r="H22">
+        <v>21</v>
+      </c>
+      <c r="I22" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23">
+        <v>49</v>
+      </c>
+      <c r="H23">
+        <v>21</v>
+      </c>
+      <c r="I23" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" t="s">
+        <v>43</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More ephyz data in DB
</commit_message>
<xml_diff>
--- a/ephyz/circuit-level-behaviors.xlsx
+++ b/ephyz/circuit-level-behaviors.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>Paper</t>
   </si>
@@ -164,6 +164,18 @@
   </si>
   <si>
     <t>GCs show ADPs in vivo to somatic stimulation, and LLDs to glomerular stimulation</t>
+  </si>
+  <si>
+    <t>Labarrera et al. (2013)</t>
+  </si>
+  <si>
+    <t>Tonic inhibition sets the state of excitability in olfactorybulb granule cells</t>
+  </si>
+  <si>
+    <t>Tonic, bulb wide inhibition</t>
+  </si>
+  <si>
+    <t>Not reported</t>
   </si>
 </sst>
 </file>
@@ -482,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,6 +730,32 @@
         <v>44</v>
       </c>
     </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" t="s">
+        <v>40</v>
+      </c>
+      <c r="J26">
+        <v>37.5</v>
+      </c>
+      <c r="K26" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>